<commit_message>
Änderung der Plot Word Funktion zum Funktionieren Außerdem herumtüfteln an dem Plot DIc Modul, welches noch nicht ganz funktioniert.
</commit_message>
<xml_diff>
--- a/Daten/Dictionaries/Dictionary asdasdf.xlsx
+++ b/Daten/Dictionaries/Dictionary asdasdf.xlsx
@@ -1,40 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jani\Documents\R Hausaufgabe\Daten\Dictionaries\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDFD245-A130-4FB2-A8F1-B407DAD33B3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">X1</t>
+    <t>Guitar</t>
   </si>
   <si>
-    <t xml:space="preserve">Guitar</t>
+    <t>Valli</t>
   </si>
   <si>
-    <t xml:space="preserve">Valli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blubbeladf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chose</t>
+    <t>Blubbeladf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,13 +64,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -351,40 +362,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>